<commit_message>
Added experiments with GAM model and tweaked plots.
</commit_message>
<xml_diff>
--- a/co2_budget_table.xlsx
+++ b/co2_budget_table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">sizecat</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grand total</t>
   </si>
 </sst>
 </file>
@@ -788,24 +785,6 @@
       <c r="I12"/>
       <c r="J12"/>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13" t="n">
-        <v>1338.62391593634</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13" t="n">
-        <v>1335.92611866219</v>
-      </c>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated and added new figure translated to english.
</commit_message>
<xml_diff>
--- a/co2_budget_table.xlsx
+++ b/co2_budget_table.xlsx
@@ -476,7 +476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -521,10 +521,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="n">
-        <v>-158.294392405132</v>
+        <v>-158.294392405131</v>
       </c>
       <c r="C2" t="n">
-        <v>28.7963691759383</v>
+        <v>28.7963691759384</v>
       </c>
       <c r="D2" t="n">
         <v>153.832343033219</v>
@@ -600,7 +600,7 @@
         <v>-174.537613180265</v>
       </c>
       <c r="C4" t="n">
-        <v>-24.0996664858583</v>
+        <v>-24.0996664858585</v>
       </c>
       <c r="D4" t="n">
         <v>71.2195855705806</v>
@@ -609,10 +609,10 @@
         <v>165.303212260541</v>
       </c>
       <c r="F4" t="n">
-        <v>332.06006013146</v>
+        <v>332.060060131461</v>
       </c>
       <c r="G4" t="n">
-        <v>72.4319819961885</v>
+        <v>72.4319819961884</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
@@ -638,7 +638,7 @@
         <v>-131.684019137498</v>
       </c>
       <c r="C5" t="n">
-        <v>-23.7825572569056</v>
+        <v>-23.7825572569055</v>
       </c>
       <c r="D5" t="n">
         <v>49.2827599727729</v>
@@ -676,7 +676,7 @@
         <v>-348.61476752094</v>
       </c>
       <c r="C6" t="n">
-        <v>-91.6764846235352</v>
+        <v>-91.6764846235354</v>
       </c>
       <c r="D6" t="n">
         <v>71.3637103243251</v>
@@ -720,7 +720,7 @@
         <v>19.9809426393038</v>
       </c>
       <c r="E7" t="n">
-        <v>77.6006308819161</v>
+        <v>77.6006308819162</v>
       </c>
       <c r="F7" t="n">
         <v>163.483747116785</v>
@@ -752,7 +752,7 @@
         <v>-213.383616186843</v>
       </c>
       <c r="C8" t="n">
-        <v>248.692074872269</v>
+        <v>248.69207487227</v>
       </c>
       <c r="D8" t="n">
         <v>574.426962526755</v>
@@ -783,10 +783,10 @@
         <v>34</v>
       </c>
       <c r="B9" t="n">
-        <v>-297.388629872211</v>
+        <v>-297.388629872212</v>
       </c>
       <c r="C9" t="n">
-        <v>-46.0111208455311</v>
+        <v>-46.0111208455312</v>
       </c>
       <c r="D9" t="n">
         <v>139.607873553316</v>
@@ -795,7 +795,7 @@
         <v>327.589027273651</v>
       </c>
       <c r="F9" t="n">
-        <v>535.794217886056</v>
+        <v>535.794217886057</v>
       </c>
       <c r="G9" t="n">
         <v>135.73123161434</v>
@@ -824,16 +824,16 @@
         <v>-1435.07573389807</v>
       </c>
       <c r="C10" t="n">
-        <v>-269.946399961938</v>
+        <v>-269.94639996194</v>
       </c>
       <c r="D10" t="n">
-        <v>410.032356937581</v>
+        <v>410.032356937582</v>
       </c>
       <c r="E10" t="n">
         <v>1119.85054625066</v>
       </c>
       <c r="F10" t="n">
-        <v>2288.85535402921</v>
+        <v>2288.85535402922</v>
       </c>
       <c r="G10" t="n">
         <v>404.036375831744</v>
@@ -859,10 +859,10 @@
         <v>41</v>
       </c>
       <c r="B11" t="n">
-        <v>-91.141267191092</v>
+        <v>-91.1412671910925</v>
       </c>
       <c r="C11" t="n">
-        <v>94.4017813310241</v>
+        <v>94.4017813310239</v>
       </c>
       <c r="D11" t="n">
         <v>228.394444540014</v>
@@ -871,7 +871,7 @@
         <v>368.623121722625</v>
       </c>
       <c r="F11" t="n">
-        <v>550.953783668845</v>
+        <v>550.953783668846</v>
       </c>
       <c r="G11" t="n">
         <v>229.623438909118</v>
@@ -897,22 +897,22 @@
         <v>31</v>
       </c>
       <c r="B12" t="n">
-        <v>-1194.38895717867</v>
+        <v>-1194.38895717868</v>
       </c>
       <c r="C12" t="n">
-        <v>66.5902658429353</v>
+        <v>66.5902658429346</v>
       </c>
       <c r="D12" t="n">
-        <v>764.196953409581</v>
+        <v>764.196953409582</v>
       </c>
       <c r="E12" t="n">
         <v>1470.15533096331</v>
       </c>
       <c r="F12" t="n">
-        <v>2694.28184616922</v>
+        <v>2694.28184616923</v>
       </c>
       <c r="G12" t="n">
-        <v>769.391046355202</v>
+        <v>769.391046355203</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>

</xml_diff>